<commit_message>
Updates roster test fixture
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_user_upload.xlsx
+++ b/spec/fixtures/test_user_upload.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylekthompson/src/osumb/challenges/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D2FBBB-7FCE-8141-84EB-75B660F0ADA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="964">
   <si>
     <t>Name</t>
   </si>
@@ -2924,8 +2925,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3017,6 +3018,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3284,14 +3288,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F244" sqref="F244"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -3303,7 +3307,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>492</v>
       </c>
@@ -3336,8 +3340,8 @@
       <c r="C2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
+      <c r="D2" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>728</v>
@@ -3349,7 +3353,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>493</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>494</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>495</v>
       </c>
@@ -3418,7 +3422,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>496</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>497</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
         <v>498</v>
       </c>
@@ -3487,7 +3491,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>499</v>
       </c>
@@ -3510,7 +3514,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>500</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>501</v>
       </c>
@@ -3556,7 +3560,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>502</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>503</v>
       </c>
@@ -3602,7 +3606,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>504</v>
       </c>
@@ -3625,7 +3629,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>505</v>
       </c>
@@ -3648,7 +3652,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
         <v>506</v>
       </c>
@@ -3671,7 +3675,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
         <v>507</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>508</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
         <v>509</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
         <v>510</v>
       </c>
@@ -3763,7 +3767,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
         <v>511</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
         <v>512</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
         <v>513</v>
       </c>
@@ -3832,7 +3836,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
         <v>514</v>
       </c>
@@ -3855,7 +3859,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="4" t="s">
         <v>515</v>
       </c>
@@ -3878,7 +3882,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="4" t="s">
         <v>516</v>
       </c>
@@ -3901,7 +3905,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="4" t="s">
         <v>517</v>
       </c>
@@ -3924,7 +3928,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="4" t="s">
         <v>518</v>
       </c>
@@ -3947,7 +3951,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
         <v>519</v>
       </c>
@@ -3970,7 +3974,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="4" t="s">
         <v>520</v>
       </c>
@@ -3993,7 +3997,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="4" t="s">
         <v>521</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
         <v>522</v>
       </c>
@@ -4039,7 +4043,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="4" t="s">
         <v>523</v>
       </c>
@@ -4062,7 +4066,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
         <v>524</v>
       </c>
@@ -4085,7 +4089,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="4" t="s">
         <v>525</v>
       </c>
@@ -4108,7 +4112,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="4" t="s">
         <v>526</v>
       </c>
@@ -4131,7 +4135,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
         <v>527</v>
       </c>
@@ -4154,7 +4158,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
         <v>528</v>
       </c>
@@ -4177,7 +4181,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="4" t="s">
         <v>529</v>
       </c>
@@ -4200,7 +4204,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="4" t="s">
         <v>530</v>
       </c>
@@ -4223,7 +4227,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>531</v>
       </c>
@@ -4246,7 +4250,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
         <v>532</v>
       </c>
@@ -4269,7 +4273,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
         <v>533</v>
       </c>
@@ -4292,7 +4296,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
         <v>534</v>
       </c>
@@ -4302,8 +4306,8 @@
       <c r="C44" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D44" s="4">
-        <v>1</v>
+      <c r="D44" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>770</v>
@@ -4315,7 +4319,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="4" t="s">
         <v>535</v>
       </c>
@@ -4325,8 +4329,8 @@
       <c r="C45" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="4">
-        <v>1</v>
+      <c r="D45" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>771</v>
@@ -4338,7 +4342,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
         <v>536</v>
       </c>
@@ -4348,8 +4352,8 @@
       <c r="C46" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D46" s="4">
-        <v>1</v>
+      <c r="D46" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>772</v>
@@ -4361,7 +4365,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="4" t="s">
         <v>537</v>
       </c>
@@ -4371,8 +4375,8 @@
       <c r="C47" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D47" s="4">
-        <v>1</v>
+      <c r="D47" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>773</v>
@@ -4384,7 +4388,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="4" t="s">
         <v>538</v>
       </c>
@@ -4394,8 +4398,8 @@
       <c r="C48" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="4">
-        <v>1</v>
+      <c r="D48" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>774</v>
@@ -4407,7 +4411,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="4" t="s">
         <v>539</v>
       </c>
@@ -4417,8 +4421,8 @@
       <c r="C49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="4">
-        <v>2</v>
+      <c r="D49" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>775</v>
@@ -4430,7 +4434,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
         <v>540</v>
       </c>
@@ -4440,8 +4444,8 @@
       <c r="C50" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D50" s="4">
-        <v>2</v>
+      <c r="D50" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>776</v>
@@ -4453,7 +4457,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
         <v>541</v>
       </c>
@@ -4463,8 +4467,8 @@
       <c r="C51" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D51" s="4">
-        <v>2</v>
+      <c r="D51" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>777</v>
@@ -4476,7 +4480,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
         <v>542</v>
       </c>
@@ -4486,8 +4490,8 @@
       <c r="C52" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="4">
-        <v>1</v>
+      <c r="D52" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>778</v>
@@ -4499,7 +4503,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="4" t="s">
         <v>543</v>
       </c>
@@ -4509,8 +4513,8 @@
       <c r="C53" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="4">
-        <v>2</v>
+      <c r="D53" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>779</v>
@@ -4522,7 +4526,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="4" t="s">
         <v>544</v>
       </c>
@@ -4532,8 +4536,8 @@
       <c r="C54" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D54" s="4">
-        <v>2</v>
+      <c r="D54" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>780</v>
@@ -4545,7 +4549,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="4" t="s">
         <v>545</v>
       </c>
@@ -4555,8 +4559,8 @@
       <c r="C55" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="4">
-        <v>2</v>
+      <c r="D55" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>781</v>
@@ -4568,7 +4572,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
         <v>546</v>
       </c>
@@ -4578,8 +4582,8 @@
       <c r="C56" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="4">
-        <v>2</v>
+      <c r="D56" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>782</v>
@@ -4591,7 +4595,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="4" t="s">
         <v>547</v>
       </c>
@@ -4601,8 +4605,8 @@
       <c r="C57" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D57" s="4">
-        <v>1</v>
+      <c r="D57" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>783</v>
@@ -4614,7 +4618,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="4" t="s">
         <v>548</v>
       </c>
@@ -4637,7 +4641,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="4" t="s">
         <v>549</v>
       </c>
@@ -4647,8 +4651,8 @@
       <c r="C59" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="4">
-        <v>2</v>
+      <c r="D59" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>785</v>
@@ -4660,7 +4664,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="4" t="s">
         <v>550</v>
       </c>
@@ -4670,8 +4674,8 @@
       <c r="C60" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D60" s="4">
-        <v>2</v>
+      <c r="D60" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>786</v>
@@ -4683,7 +4687,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="4" t="s">
         <v>551</v>
       </c>
@@ -4693,8 +4697,8 @@
       <c r="C61" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="4">
-        <v>1</v>
+      <c r="D61" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>787</v>
@@ -4706,7 +4710,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="4" t="s">
         <v>552</v>
       </c>
@@ -4716,8 +4720,8 @@
       <c r="C62" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D62" s="4">
-        <v>2</v>
+      <c r="D62" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>788</v>
@@ -4730,7 +4734,7 @@
       </c>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="4" t="s">
         <v>553</v>
       </c>
@@ -4753,7 +4757,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="4" t="s">
         <v>554</v>
       </c>
@@ -4763,8 +4767,8 @@
       <c r="C64" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D64" s="4">
-        <v>1</v>
+      <c r="D64" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>790</v>
@@ -4776,7 +4780,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="4" t="s">
         <v>555</v>
       </c>
@@ -4786,8 +4790,8 @@
       <c r="C65" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D65" s="4">
-        <v>2</v>
+      <c r="D65" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>791</v>
@@ -4799,7 +4803,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="4" t="s">
         <v>556</v>
       </c>
@@ -4822,7 +4826,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="4" t="s">
         <v>557</v>
       </c>
@@ -4832,8 +4836,8 @@
       <c r="C67" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="4">
-        <v>1</v>
+      <c r="D67" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>793</v>
@@ -4845,7 +4849,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" s="4" t="s">
         <v>558</v>
       </c>
@@ -4855,8 +4859,8 @@
       <c r="C68" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D68" s="4">
-        <v>2</v>
+      <c r="D68" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>794</v>
@@ -4868,7 +4872,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" s="4" t="s">
         <v>559</v>
       </c>
@@ -4878,8 +4882,8 @@
       <c r="C69" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D69" s="4">
-        <v>1</v>
+      <c r="D69" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>795</v>
@@ -4891,7 +4895,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" s="4" t="s">
         <v>560</v>
       </c>
@@ -4901,8 +4905,8 @@
       <c r="C70" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D70" s="4">
-        <v>1</v>
+      <c r="D70" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>796</v>
@@ -4914,7 +4918,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" s="4" t="s">
         <v>561</v>
       </c>
@@ -4937,7 +4941,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" s="4" t="s">
         <v>562</v>
       </c>
@@ -4958,7 +4962,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" s="4" t="s">
         <v>563</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" s="4" t="s">
         <v>564</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" s="4" t="s">
         <v>565</v>
       </c>
@@ -5021,7 +5025,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="4" t="s">
         <v>566</v>
       </c>
@@ -5042,7 +5046,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" s="4" t="s">
         <v>567</v>
       </c>
@@ -5063,7 +5067,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" s="4" t="s">
         <v>568</v>
       </c>
@@ -5084,7 +5088,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" s="4" t="s">
         <v>569</v>
       </c>
@@ -5105,7 +5109,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="4" t="s">
         <v>570</v>
       </c>
@@ -5126,7 +5130,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" s="4" t="s">
         <v>571</v>
       </c>
@@ -5147,7 +5151,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" s="4" t="s">
         <v>572</v>
       </c>
@@ -5168,7 +5172,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" s="4" t="s">
         <v>573</v>
       </c>
@@ -5189,7 +5193,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" s="4" t="s">
         <v>574</v>
       </c>
@@ -5210,7 +5214,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" s="4" t="s">
         <v>575</v>
       </c>
@@ -5231,7 +5235,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" s="4" t="s">
         <v>576</v>
       </c>
@@ -5254,7 +5258,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" s="4" t="s">
         <v>577</v>
       </c>
@@ -5277,7 +5281,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" s="4" t="s">
         <v>578</v>
       </c>
@@ -5300,7 +5304,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" s="4" t="s">
         <v>579</v>
       </c>
@@ -5323,7 +5327,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" s="4" t="s">
         <v>580</v>
       </c>
@@ -5346,7 +5350,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" s="4" t="s">
         <v>581</v>
       </c>
@@ -5369,7 +5373,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" s="4" t="s">
         <v>582</v>
       </c>
@@ -5392,7 +5396,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" s="4" t="s">
         <v>583</v>
       </c>
@@ -5415,7 +5419,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" s="4" t="s">
         <v>584</v>
       </c>
@@ -5438,7 +5442,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" s="4" t="s">
         <v>585</v>
       </c>
@@ -5461,7 +5465,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" s="4" t="s">
         <v>586</v>
       </c>
@@ -5484,7 +5488,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" s="4" t="s">
         <v>587</v>
       </c>
@@ -5507,7 +5511,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" s="4" t="s">
         <v>588</v>
       </c>
@@ -5530,7 +5534,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" s="4" t="s">
         <v>589</v>
       </c>
@@ -5553,7 +5557,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" s="4" t="s">
         <v>590</v>
       </c>
@@ -5576,7 +5580,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" s="4" t="s">
         <v>591</v>
       </c>
@@ -5599,7 +5603,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" s="4" t="s">
         <v>592</v>
       </c>
@@ -5622,7 +5626,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" s="4" t="s">
         <v>593</v>
       </c>
@@ -5645,7 +5649,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" s="4" t="s">
         <v>594</v>
       </c>
@@ -5668,7 +5672,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" s="4" t="s">
         <v>595</v>
       </c>
@@ -5691,7 +5695,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" s="4" t="s">
         <v>596</v>
       </c>
@@ -5714,7 +5718,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" s="4" t="s">
         <v>597</v>
       </c>
@@ -5737,7 +5741,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" s="4" t="s">
         <v>598</v>
       </c>
@@ -5760,7 +5764,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" s="4" t="s">
         <v>599</v>
       </c>
@@ -5783,7 +5787,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" s="4" t="s">
         <v>600</v>
       </c>
@@ -5806,7 +5810,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" s="4" t="s">
         <v>601</v>
       </c>
@@ -5829,7 +5833,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" s="4" t="s">
         <v>602</v>
       </c>
@@ -5852,7 +5856,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" s="4" t="s">
         <v>603</v>
       </c>
@@ -5875,7 +5879,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" s="4" t="s">
         <v>604</v>
       </c>
@@ -5898,7 +5902,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" s="4" t="s">
         <v>605</v>
       </c>
@@ -5921,7 +5925,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" s="4" t="s">
         <v>606</v>
       </c>
@@ -5944,7 +5948,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" s="4" t="s">
         <v>607</v>
       </c>
@@ -5967,7 +5971,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" s="4" t="s">
         <v>608</v>
       </c>
@@ -5988,7 +5992,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" s="4" t="s">
         <v>609</v>
       </c>
@@ -6009,7 +6013,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" s="4" t="s">
         <v>610</v>
       </c>
@@ -6030,7 +6034,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" s="4" t="s">
         <v>611</v>
       </c>
@@ -6051,7 +6055,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" s="4" t="s">
         <v>612</v>
       </c>
@@ -6072,7 +6076,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" s="4" t="s">
         <v>613</v>
       </c>
@@ -6093,7 +6097,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" s="4" t="s">
         <v>614</v>
       </c>
@@ -6114,7 +6118,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7">
       <c r="A125" s="4" t="s">
         <v>615</v>
       </c>
@@ -6135,7 +6139,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="A126" s="4" t="s">
         <v>616</v>
       </c>
@@ -6156,7 +6160,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7">
       <c r="A127" s="4" t="s">
         <v>617</v>
       </c>
@@ -6177,7 +6181,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128" s="4" t="s">
         <v>618</v>
       </c>
@@ -6198,7 +6202,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7">
       <c r="A129" s="4" t="s">
         <v>619</v>
       </c>
@@ -6219,7 +6223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7">
       <c r="A130" s="4" t="s">
         <v>620</v>
       </c>
@@ -6240,7 +6244,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7">
       <c r="A131" s="4" t="s">
         <v>621</v>
       </c>
@@ -6261,7 +6265,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7">
       <c r="A132" s="4" t="s">
         <v>622</v>
       </c>
@@ -6282,7 +6286,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7">
       <c r="A133" s="4" t="s">
         <v>623</v>
       </c>
@@ -6303,7 +6307,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7">
       <c r="A134" s="4" t="s">
         <v>624</v>
       </c>
@@ -6324,7 +6328,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7">
       <c r="A135" s="4" t="s">
         <v>625</v>
       </c>
@@ -6345,7 +6349,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7">
       <c r="A136" s="4" t="s">
         <v>626</v>
       </c>
@@ -6366,7 +6370,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7">
       <c r="A137" s="4" t="s">
         <v>627</v>
       </c>
@@ -6387,7 +6391,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7">
       <c r="A138" s="4" t="s">
         <v>628</v>
       </c>
@@ -6408,7 +6412,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7">
       <c r="A139" s="4" t="s">
         <v>629</v>
       </c>
@@ -6429,7 +6433,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7">
       <c r="A140" s="4" t="s">
         <v>630</v>
       </c>
@@ -6450,7 +6454,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7">
       <c r="A141" s="4" t="s">
         <v>631</v>
       </c>
@@ -6471,7 +6475,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7">
       <c r="A142" s="4" t="s">
         <v>632</v>
       </c>
@@ -6492,7 +6496,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7">
       <c r="A143" s="4" t="s">
         <v>633</v>
       </c>
@@ -6513,7 +6517,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7">
       <c r="A144" s="4" t="s">
         <v>634</v>
       </c>
@@ -6534,7 +6538,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7">
       <c r="A145" s="4" t="s">
         <v>635</v>
       </c>
@@ -6555,7 +6559,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7">
       <c r="A146" s="4" t="s">
         <v>636</v>
       </c>
@@ -6576,7 +6580,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7">
       <c r="A147" s="4" t="s">
         <v>637</v>
       </c>
@@ -6597,7 +6601,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7">
       <c r="A148" s="4" t="s">
         <v>638</v>
       </c>
@@ -6618,7 +6622,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7">
       <c r="A149" s="4" t="s">
         <v>639</v>
       </c>
@@ -6639,7 +6643,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7">
       <c r="A150" s="4" t="s">
         <v>640</v>
       </c>
@@ -6660,7 +6664,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7">
       <c r="A151" s="4" t="s">
         <v>641</v>
       </c>
@@ -6681,7 +6685,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7">
       <c r="A152" s="4" t="s">
         <v>642</v>
       </c>
@@ -6702,7 +6706,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7">
       <c r="A153" s="4" t="s">
         <v>643</v>
       </c>
@@ -6723,7 +6727,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7">
       <c r="A154" s="4" t="s">
         <v>644</v>
       </c>
@@ -6744,7 +6748,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7">
       <c r="A155" s="4" t="s">
         <v>645</v>
       </c>
@@ -6765,7 +6769,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7">
       <c r="A156" s="4" t="s">
         <v>646</v>
       </c>
@@ -6786,7 +6790,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7">
       <c r="A157" s="4" t="s">
         <v>647</v>
       </c>
@@ -6807,7 +6811,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7">
       <c r="A158" s="4" t="s">
         <v>648</v>
       </c>
@@ -6828,7 +6832,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7">
       <c r="A159" s="4" t="s">
         <v>649</v>
       </c>
@@ -6849,7 +6853,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7">
       <c r="A160" s="4" t="s">
         <v>650</v>
       </c>
@@ -6859,8 +6863,8 @@
       <c r="C160" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D160" s="4">
-        <v>2</v>
+      <c r="D160" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E160" s="4" t="s">
         <v>886</v>
@@ -6872,7 +6876,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7">
       <c r="A161" s="4" t="s">
         <v>651</v>
       </c>
@@ -6882,8 +6886,8 @@
       <c r="C161" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D161" s="4">
-        <v>1</v>
+      <c r="D161" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>887</v>
@@ -6895,7 +6899,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7">
       <c r="A162" s="4" t="s">
         <v>652</v>
       </c>
@@ -6906,7 +6910,7 @@
         <v>89</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="E162" s="4" t="s">
         <v>888</v>
@@ -6918,7 +6922,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7">
       <c r="A163" s="4" t="s">
         <v>653</v>
       </c>
@@ -6928,8 +6932,8 @@
       <c r="C163" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D163" s="4">
-        <v>2</v>
+      <c r="D163" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>889</v>
@@ -6941,7 +6945,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7">
       <c r="A164" s="4" t="s">
         <v>654</v>
       </c>
@@ -6951,8 +6955,8 @@
       <c r="C164" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D164" s="4">
-        <v>1</v>
+      <c r="D164" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E164" s="4" t="s">
         <v>890</v>
@@ -6964,7 +6968,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7">
       <c r="A165" s="4" t="s">
         <v>655</v>
       </c>
@@ -6974,8 +6978,8 @@
       <c r="C165" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D165" s="4">
-        <v>2</v>
+      <c r="D165" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>891</v>
@@ -6987,7 +6991,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7">
       <c r="A166" s="4" t="s">
         <v>656</v>
       </c>
@@ -6997,8 +7001,8 @@
       <c r="C166" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D166" s="4">
-        <v>1</v>
+      <c r="D166" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E166" s="4" t="s">
         <v>892</v>
@@ -7010,7 +7014,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7">
       <c r="A167" s="4" t="s">
         <v>657</v>
       </c>
@@ -7020,8 +7024,8 @@
       <c r="C167" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="D167" s="4">
-        <v>2</v>
+      <c r="D167" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>893</v>
@@ -7033,7 +7037,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7">
       <c r="A168" s="4" t="s">
         <v>658</v>
       </c>
@@ -7056,7 +7060,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7">
       <c r="A169" s="4" t="s">
         <v>659</v>
       </c>
@@ -7066,8 +7070,8 @@
       <c r="C169" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D169" s="4">
-        <v>1</v>
+      <c r="D169" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>895</v>
@@ -7079,7 +7083,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7">
       <c r="A170" s="4" t="s">
         <v>660</v>
       </c>
@@ -7089,8 +7093,8 @@
       <c r="C170" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D170" s="4">
-        <v>2</v>
+      <c r="D170" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E170" s="4" t="s">
         <v>896</v>
@@ -7102,7 +7106,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7">
       <c r="A171" s="4" t="s">
         <v>661</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>24</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>13</v>
+        <v>246</v>
       </c>
       <c r="E171" s="4" t="s">
         <v>897</v>
@@ -7125,7 +7129,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7">
       <c r="A172" s="4" t="s">
         <v>662</v>
       </c>
@@ -7135,8 +7139,8 @@
       <c r="C172" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D172" s="4">
-        <v>1</v>
+      <c r="D172" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E172" s="4" t="s">
         <v>898</v>
@@ -7148,7 +7152,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7">
       <c r="A173" s="4" t="s">
         <v>663</v>
       </c>
@@ -7158,8 +7162,8 @@
       <c r="C173" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D173" s="4">
-        <v>2</v>
+      <c r="D173" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E173" s="4" t="s">
         <v>899</v>
@@ -7171,7 +7175,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7">
       <c r="A174" s="4" t="s">
         <v>664</v>
       </c>
@@ -7181,8 +7185,8 @@
       <c r="C174" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D174" s="4">
-        <v>1</v>
+      <c r="D174" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E174" s="4" t="s">
         <v>900</v>
@@ -7194,7 +7198,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7">
       <c r="A175" s="4" t="s">
         <v>665</v>
       </c>
@@ -7204,8 +7208,8 @@
       <c r="C175" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D175" s="4">
-        <v>2</v>
+      <c r="D175" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E175" s="4" t="s">
         <v>901</v>
@@ -7217,7 +7221,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7">
       <c r="A176" s="4" t="s">
         <v>666</v>
       </c>
@@ -7227,8 +7231,8 @@
       <c r="C176" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D176" s="4">
-        <v>1</v>
+      <c r="D176" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E176" s="4" t="s">
         <v>902</v>
@@ -7240,7 +7244,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7">
       <c r="A177" s="4" t="s">
         <v>667</v>
       </c>
@@ -7250,8 +7254,8 @@
       <c r="C177" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D177" s="4">
-        <v>1</v>
+      <c r="D177" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>903</v>
@@ -7263,7 +7267,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7">
       <c r="A178" s="4" t="s">
         <v>668</v>
       </c>
@@ -7273,8 +7277,8 @@
       <c r="C178" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D178" s="4">
-        <v>2</v>
+      <c r="D178" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E178" s="4" t="s">
         <v>904</v>
@@ -7286,7 +7290,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7">
       <c r="A179" s="4" t="s">
         <v>669</v>
       </c>
@@ -7296,8 +7300,8 @@
       <c r="C179" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D179" s="4">
-        <v>1</v>
+      <c r="D179" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E179" s="4" t="s">
         <v>905</v>
@@ -7309,7 +7313,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7">
       <c r="A180" s="4" t="s">
         <v>670</v>
       </c>
@@ -7319,8 +7323,8 @@
       <c r="C180" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D180" s="4">
-        <v>2</v>
+      <c r="D180" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E180" s="4" t="s">
         <v>906</v>
@@ -7332,7 +7336,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7">
       <c r="A181" s="4" t="s">
         <v>671</v>
       </c>
@@ -7342,8 +7346,8 @@
       <c r="C181" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D181" s="4">
-        <v>2</v>
+      <c r="D181" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E181" s="4" t="s">
         <v>907</v>
@@ -7355,7 +7359,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7">
       <c r="A182" s="4" t="s">
         <v>672</v>
       </c>
@@ -7365,8 +7369,8 @@
       <c r="C182" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D182" s="4">
-        <v>1</v>
+      <c r="D182" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E182" s="4" t="s">
         <v>908</v>
@@ -7378,7 +7382,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7">
       <c r="A183" s="4" t="s">
         <v>673</v>
       </c>
@@ -7388,8 +7392,8 @@
       <c r="C183" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D183" s="4">
-        <v>2</v>
+      <c r="D183" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E183" s="4" t="s">
         <v>909</v>
@@ -7401,7 +7405,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7">
       <c r="A184" s="4" t="s">
         <v>674</v>
       </c>
@@ -7411,8 +7415,8 @@
       <c r="C184" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D184" s="4">
-        <v>1</v>
+      <c r="D184" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E184" s="4" t="s">
         <v>910</v>
@@ -7424,7 +7428,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7">
       <c r="A185" s="4" t="s">
         <v>675</v>
       </c>
@@ -7434,8 +7438,8 @@
       <c r="C185" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D185" s="4">
-        <v>2</v>
+      <c r="D185" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E185" s="4" t="s">
         <v>911</v>
@@ -7447,7 +7451,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7">
       <c r="A186" s="4" t="s">
         <v>676</v>
       </c>
@@ -7457,8 +7461,8 @@
       <c r="C186" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D186" s="4">
-        <v>1</v>
+      <c r="D186" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E186" s="4" t="s">
         <v>912</v>
@@ -7470,7 +7474,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7">
       <c r="A187" s="4" t="s">
         <v>677</v>
       </c>
@@ -7480,8 +7484,8 @@
       <c r="C187" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D187" s="4">
-        <v>2</v>
+      <c r="D187" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E187" s="4" t="s">
         <v>913</v>
@@ -7493,7 +7497,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7">
       <c r="A188" s="4" t="s">
         <v>678</v>
       </c>
@@ -7516,7 +7520,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7">
       <c r="A189" s="4" t="s">
         <v>679</v>
       </c>
@@ -7526,8 +7530,8 @@
       <c r="C189" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D189" s="4">
-        <v>2</v>
+      <c r="D189" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E189" s="4" t="s">
         <v>915</v>
@@ -7539,7 +7543,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7">
       <c r="A190" s="4" t="s">
         <v>680</v>
       </c>
@@ -7562,7 +7566,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7">
       <c r="A191" s="4" t="s">
         <v>681</v>
       </c>
@@ -7572,8 +7576,8 @@
       <c r="C191" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D191" s="4">
-        <v>2</v>
+      <c r="D191" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E191" s="4" t="s">
         <v>917</v>
@@ -7585,7 +7589,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7">
       <c r="A192" s="4" t="s">
         <v>682</v>
       </c>
@@ -7608,7 +7612,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7">
       <c r="A193" s="4" t="s">
         <v>683</v>
       </c>
@@ -7618,8 +7622,8 @@
       <c r="C193" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D193" s="4">
-        <v>2</v>
+      <c r="D193" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E193" s="4" t="s">
         <v>919</v>
@@ -7631,7 +7635,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7">
       <c r="A194" s="4" t="s">
         <v>684</v>
       </c>
@@ -7641,8 +7645,8 @@
       <c r="C194" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D194" s="4">
-        <v>2</v>
+      <c r="D194" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E194" s="4" t="s">
         <v>920</v>
@@ -7654,7 +7658,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7">
       <c r="A195" s="4" t="s">
         <v>685</v>
       </c>
@@ -7677,7 +7681,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7">
       <c r="A196" s="4" t="s">
         <v>686</v>
       </c>
@@ -7687,8 +7691,8 @@
       <c r="C196" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D196" s="4">
-        <v>2</v>
+      <c r="D196" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E196" s="4" t="s">
         <v>922</v>
@@ -7700,7 +7704,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7">
       <c r="A197" s="4" t="s">
         <v>687</v>
       </c>
@@ -7723,7 +7727,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7">
       <c r="A198" s="4" t="s">
         <v>688</v>
       </c>
@@ -7733,8 +7737,8 @@
       <c r="C198" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D198" s="4">
-        <v>2</v>
+      <c r="D198" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E198" s="4" t="s">
         <v>924</v>
@@ -7746,7 +7750,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7">
       <c r="A199" s="4" t="s">
         <v>689</v>
       </c>
@@ -7769,7 +7773,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7">
       <c r="A200" s="4" t="s">
         <v>690</v>
       </c>
@@ -7792,7 +7796,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7">
       <c r="A201" s="4" t="s">
         <v>691</v>
       </c>
@@ -7802,8 +7806,8 @@
       <c r="C201" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D201" s="4">
-        <v>2</v>
+      <c r="D201" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E201" s="4" t="s">
         <v>927</v>
@@ -7815,7 +7819,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7">
       <c r="A202" s="4" t="s">
         <v>692</v>
       </c>
@@ -7825,8 +7829,8 @@
       <c r="C202" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D202" s="4">
-        <v>2</v>
+      <c r="D202" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E202" s="4" t="s">
         <v>928</v>
@@ -7838,7 +7842,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7">
       <c r="A203" s="4" t="s">
         <v>693</v>
       </c>
@@ -7848,8 +7852,8 @@
       <c r="C203" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D203" s="4">
-        <v>2</v>
+      <c r="D203" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E203" s="4" t="s">
         <v>929</v>
@@ -7861,7 +7865,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7">
       <c r="A204" s="4" t="s">
         <v>694</v>
       </c>
@@ -7871,8 +7875,8 @@
       <c r="C204" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D204" s="4">
-        <v>1</v>
+      <c r="D204" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E204" s="4" t="s">
         <v>930</v>
@@ -7884,7 +7888,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7">
       <c r="A205" s="4" t="s">
         <v>695</v>
       </c>
@@ -7894,8 +7898,8 @@
       <c r="C205" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D205" s="4">
-        <v>2</v>
+      <c r="D205" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E205" s="4" t="s">
         <v>931</v>
@@ -7907,7 +7911,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7">
       <c r="A206" s="4" t="s">
         <v>696</v>
       </c>
@@ -7917,8 +7921,8 @@
       <c r="C206" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D206" s="4">
-        <v>1</v>
+      <c r="D206" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E206" s="4" t="s">
         <v>932</v>
@@ -7930,7 +7934,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7">
       <c r="A207" s="4" t="s">
         <v>697</v>
       </c>
@@ -7940,8 +7944,8 @@
       <c r="C207" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D207" s="4">
-        <v>2</v>
+      <c r="D207" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E207" s="4" t="s">
         <v>933</v>
@@ -7953,7 +7957,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7">
       <c r="A208" s="4" t="s">
         <v>698</v>
       </c>
@@ -7963,8 +7967,8 @@
       <c r="C208" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D208" s="4">
-        <v>1</v>
+      <c r="D208" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E208" s="4" t="s">
         <v>934</v>
@@ -7976,7 +7980,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7">
       <c r="A209" s="4" t="s">
         <v>699</v>
       </c>
@@ -7986,8 +7990,8 @@
       <c r="C209" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D209" s="4">
-        <v>2</v>
+      <c r="D209" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E209" s="4" t="s">
         <v>935</v>
@@ -7999,7 +8003,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7">
       <c r="A210" s="4" t="s">
         <v>700</v>
       </c>
@@ -8009,8 +8013,8 @@
       <c r="C210" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D210" s="4">
-        <v>1</v>
+      <c r="D210" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E210" s="4" t="s">
         <v>936</v>
@@ -8022,7 +8026,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7">
       <c r="A211" s="4" t="s">
         <v>701</v>
       </c>
@@ -8032,8 +8036,8 @@
       <c r="C211" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D211" s="4">
-        <v>1</v>
+      <c r="D211" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E211" s="4" t="s">
         <v>937</v>
@@ -8045,7 +8049,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7">
       <c r="A212" s="4" t="s">
         <v>702</v>
       </c>
@@ -8055,8 +8059,8 @@
       <c r="C212" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D212" s="4">
-        <v>2</v>
+      <c r="D212" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E212" s="4" t="s">
         <v>938</v>
@@ -8068,7 +8072,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7">
       <c r="A213" s="4" t="s">
         <v>703</v>
       </c>
@@ -8078,8 +8082,8 @@
       <c r="C213" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D213" s="4">
-        <v>2</v>
+      <c r="D213" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E213" s="4" t="s">
         <v>939</v>
@@ -8091,7 +8095,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7">
       <c r="A214" s="4" t="s">
         <v>704</v>
       </c>
@@ -8101,8 +8105,8 @@
       <c r="C214" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D214" s="4">
-        <v>1</v>
+      <c r="D214" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E214" s="4" t="s">
         <v>940</v>
@@ -8114,7 +8118,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7">
       <c r="A215" s="4" t="s">
         <v>705</v>
       </c>
@@ -8124,8 +8128,8 @@
       <c r="C215" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D215" s="4">
-        <v>2</v>
+      <c r="D215" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="E215" s="4" t="s">
         <v>941</v>
@@ -8137,7 +8141,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7">
       <c r="A216" s="4" t="s">
         <v>706</v>
       </c>
@@ -8160,7 +8164,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7">
       <c r="A217" s="4" t="s">
         <v>707</v>
       </c>
@@ -8183,7 +8187,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7">
       <c r="A218" s="4" t="s">
         <v>708</v>
       </c>
@@ -8206,7 +8210,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7">
       <c r="A219" s="4" t="s">
         <v>709</v>
       </c>
@@ -8229,7 +8233,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7">
       <c r="A220" s="4" t="s">
         <v>710</v>
       </c>
@@ -8252,7 +8256,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7">
       <c r="A221" s="4" t="s">
         <v>711</v>
       </c>
@@ -8275,7 +8279,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7">
       <c r="A222" s="4" t="s">
         <v>712</v>
       </c>
@@ -8298,7 +8302,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7">
       <c r="A223" s="4" t="s">
         <v>713</v>
       </c>
@@ -8321,7 +8325,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7">
       <c r="A224" s="4" t="s">
         <v>714</v>
       </c>
@@ -8344,7 +8348,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7">
       <c r="A225" s="4" t="s">
         <v>715</v>
       </c>
@@ -8367,7 +8371,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7">
       <c r="A226" s="4" t="s">
         <v>716</v>
       </c>
@@ -8390,7 +8394,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7">
       <c r="A227" s="4" t="s">
         <v>717</v>
       </c>
@@ -8413,7 +8417,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7">
       <c r="A228" s="4" t="s">
         <v>718</v>
       </c>
@@ -8436,7 +8440,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7">
       <c r="A229" s="4" t="s">
         <v>719</v>
       </c>
@@ -8459,7 +8463,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7">
       <c r="A230" s="4" t="s">
         <v>720</v>
       </c>
@@ -8480,7 +8484,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7">
       <c r="A231" s="4" t="s">
         <v>721</v>
       </c>
@@ -8501,7 +8505,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7">
       <c r="A232" s="4" t="s">
         <v>722</v>
       </c>
@@ -8522,7 +8526,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7">
       <c r="A233" s="4" t="s">
         <v>723</v>
       </c>
@@ -8543,7 +8547,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7">
       <c r="A234" s="4" t="s">
         <v>724</v>
       </c>
@@ -8564,7 +8568,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7">
       <c r="A235" s="4" t="s">
         <v>725</v>
       </c>
@@ -8585,7 +8589,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7">
       <c r="A236" s="4" t="s">
         <v>726</v>
       </c>
@@ -8606,7 +8610,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7">
       <c r="A237" s="4" t="s">
         <v>727</v>
       </c>
@@ -8627,14 +8631,14 @@
         <v>255</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7">
       <c r="A238" s="3"/>
       <c r="B238" s="3"/>
       <c r="E238" s="6"/>
       <c r="F238" s="7"/>
       <c r="G238" s="2"/>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7">
       <c r="A239" s="3"/>
       <c r="B239" s="3"/>
       <c r="E239" s="6"/>

</xml_diff>